<commit_message>
Report and evidence excel for Assignment 4
</commit_message>
<xml_diff>
--- a/INFO6205/Assignment4/Assignment4_002772160.xlsx
+++ b/INFO6205/Assignment4/Assignment4_002772160.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shivanidatar/Documents/6205/PSA-Git/info6205-psa/INFO6205/Assignment4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD46801F-875D-894A-BDE1-ECA7333C80F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF004630-5DED-4445-86A3-36B4DA847116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16700" xr2:uid="{0B3556F7-AC56-5643-AF68-BCFBDFFC9E1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>N(total number of objects)</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>*---- To check the relationship eqivalency -------*</t>
+  </si>
+  <si>
+    <t>c = m/n log n</t>
   </si>
 </sst>
 </file>
@@ -148,13 +151,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Relationship</a:t>
+              <a:t>Relationship between number of objects and number of pairs generated</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> between number of objects and number of pairs generated</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1082,14 +1080,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
+      <xdr:colOff>139700</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1418,7 +1416,7 @@
   <dimension ref="C3:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1444,7 +1442,7 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.2">

</xml_diff>